<commit_message>
adding XML taks in the minimalistic example; small fix
</commit_message>
<xml_diff>
--- a/examples/simple/simple.xlsx
+++ b/examples/simple/simple.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jose/Documents/Research/projects/valu3s/wip/uppx/examples/simple/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36EB03B-FB37-CA46-9248-CF58F965850A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBDE590-F829-2F4D-87D6-F63B0DE44E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{F23A7857-2A5B-744A-861E-37E01B360061}"/>
   </bookViews>
   <sheets>
     <sheet name="@Channels" sheetId="12" r:id="rId1"/>
     <sheet name="@Limits" sheetId="6" r:id="rId2"/>
-    <sheet name="AvailableFunctions" sheetId="13" r:id="rId3"/>
+    <sheet name="&lt;queries&gt;" sheetId="14" r:id="rId3"/>
+    <sheet name="AvailableFunctions" sheetId="13" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="186">
   <si>
     <t>Comment</t>
   </si>
@@ -558,6 +559,45 @@
   </si>
   <si>
     <t>YEAR</t>
+  </si>
+  <si>
+    <t>&lt;query&gt;
+  &lt;formula&gt;$Formula&lt;/formula&gt;
+  &lt;comment&gt;$Comment&lt;/comment&gt;
+&lt;/query&gt;</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>NoDL</t>
+  </si>
+  <si>
+    <t>A[]!deadlock</t>
+  </si>
+  <si>
+    <t>No deadlocks</t>
+  </si>
+  <si>
+    <t>A[] W.Idle</t>
+  </si>
+  <si>
+    <t>Idle worker</t>
+  </si>
+  <si>
+    <t>Idle hammer</t>
+  </si>
+  <si>
+    <t>E&lt;&gt; H.Idle</t>
+  </si>
+  <si>
+    <t>The worker is always Idle</t>
+  </si>
+  <si>
+    <t>The hammer can be Idle</t>
+  </si>
+  <si>
+    <t>Formula</t>
   </si>
 </sst>
 </file>
@@ -623,7 +663,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -643,6 +683,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1135,6 +1176,72 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E766410-42AB-D842-913C-A2316B1EA100}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="30.83203125" customWidth="1"/>
+    <col min="3" max="3" width="25.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC6D41BA-2AFD-1444-8964-7539D3436D4A}">
   <dimension ref="A1:A160"/>
   <sheetViews>
@@ -1948,21 +2055,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DA12DE6878FEE740AAE11B8EF5A3BEB8" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ccf3f071624932fa9b6b142dc8790e1c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf33d030-a745-437b-8efe-493a0e84c7f1" xmlns:ns3="38766943-c6ee-43fb-a1f1-f050a673c741" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="46fa4806b78295368f283e4cef5efe23" ns2:_="" ns3:_="">
     <xsd:import namespace="bf33d030-a745-437b-8efe-493a0e84c7f1"/>
@@ -2173,10 +2265,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A07F53CA-6B4E-4B2E-8600-AB0859BD2077}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{030D8A7F-6A3B-4D41-86D3-C760184B49E7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bf33d030-a745-437b-8efe-493a0e84c7f1"/>
+    <ds:schemaRef ds:uri="38766943-c6ee-43fb-a1f1-f050a673c741"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2199,20 +2317,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{030D8A7F-6A3B-4D41-86D3-C760184B49E7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A07F53CA-6B4E-4B2E-8600-AB0859BD2077}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="bf33d030-a745-437b-8efe-493a0e84c7f1"/>
-    <ds:schemaRef ds:uri="38766943-c6ee-43fb-a1f1-f050a673c741"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixed unsorted messages when running checks
</commit_message>
<xml_diff>
--- a/examples/simple/simple.xlsx
+++ b/examples/simple/simple.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jose/Documents/Research/projects/valu3s/wip/uppx/examples/simple/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBDE590-F829-2F4D-87D6-F63B0DE44E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24A5958-B1A1-7744-A74F-D908332E52C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{F23A7857-2A5B-744A-861E-37E01B360061}"/>
   </bookViews>
@@ -683,7 +683,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1179,7 +1181,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E766410-42AB-D842-913C-A2316B1EA100}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1187,7 +1191,7 @@
     <col min="3" max="3" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="187" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>174</v>
       </c>
@@ -1238,6 +1242,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2055,6 +2060,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DA12DE6878FEE740AAE11B8EF5A3BEB8" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ccf3f071624932fa9b6b142dc8790e1c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf33d030-a745-437b-8efe-493a0e84c7f1" xmlns:ns3="38766943-c6ee-43fb-a1f1-f050a673c741" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="46fa4806b78295368f283e4cef5efe23" ns2:_="" ns3:_="">
     <xsd:import namespace="bf33d030-a745-437b-8efe-493a0e84c7f1"/>
@@ -2265,36 +2285,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{030D8A7F-6A3B-4D41-86D3-C760184B49E7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A07F53CA-6B4E-4B2E-8600-AB0859BD2077}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="bf33d030-a745-437b-8efe-493a0e84c7f1"/>
-    <ds:schemaRef ds:uri="38766943-c6ee-43fb-a1f1-f050a673c741"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2317,9 +2311,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A07F53CA-6B4E-4B2E-8600-AB0859BD2077}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{030D8A7F-6A3B-4D41-86D3-C760184B49E7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bf33d030-a745-437b-8efe-493a0e84c7f1"/>
+    <ds:schemaRef ds:uri="38766943-c6ee-43fb-a1f1-f050a673c741"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>